<commit_message>
cap nhat tai lieu
cap nhat tai lieu
</commit_message>
<xml_diff>
--- a/tools/IP-Planning-Hardware-Requirements.xlsx
+++ b/tools/IP-Planning-Hardware-Requirements.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CEPH-Alone" sheetId="7" r:id="rId1"/>
     <sheet name="OpenStack_Ceph-AIO-Ubuntu" sheetId="8" r:id="rId2"/>
     <sheet name="OpenStack_Ceph-AIO-CentOS" sheetId="9" r:id="rId3"/>
+    <sheet name="OpenStack_Pike" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="65">
   <si>
     <t>Controller</t>
   </si>
@@ -167,6 +168,66 @@
   </si>
   <si>
     <t>10.10.30.71</t>
+  </si>
+  <si>
+    <t>IP PLANNING - OpenStack Pike</t>
+  </si>
+  <si>
+    <t>ens160</t>
+  </si>
+  <si>
+    <t>ens192</t>
+  </si>
+  <si>
+    <t>ens224</t>
+  </si>
+  <si>
+    <t>192.168.20.44</t>
+  </si>
+  <si>
+    <t>172.16.20.44</t>
+  </si>
+  <si>
+    <t>192.168.20.254</t>
+  </si>
+  <si>
+    <t>192.168.40.44</t>
+  </si>
+  <si>
+    <t>192.168.20.45</t>
+  </si>
+  <si>
+    <t>172.16.20.45</t>
+  </si>
+  <si>
+    <t>192.168.40.45</t>
+  </si>
+  <si>
+    <t>192.168.20.46</t>
+  </si>
+  <si>
+    <t>172.16.20.46</t>
+  </si>
+  <si>
+    <t>192.168.40.46</t>
+  </si>
+  <si>
+    <t>+60</t>
+  </si>
+  <si>
+    <t>+40</t>
+  </si>
+  <si>
+    <t>Net</t>
+  </si>
+  <si>
+    <t>Bridge</t>
+  </si>
+  <si>
+    <t>Hostonly</t>
+  </si>
+  <si>
+    <t>NAT</t>
   </si>
 </sst>
 </file>
@@ -209,7 +270,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -258,6 +319,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -422,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -507,6 +574,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -516,12 +592,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -540,7 +616,13 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -552,16 +634,73 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -863,23 +1002,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="42"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="45"/>
     </row>
     <row r="3" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
@@ -923,7 +1062,7 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -937,30 +1076,30 @@
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="43">
-        <v>4</v>
-      </c>
-      <c r="I4" s="43">
+      <c r="H4" s="38">
+        <v>4</v>
+      </c>
+      <c r="I4" s="38">
         <v>2</v>
       </c>
-      <c r="J4" s="35">
+      <c r="J4" s="39">
         <v>40</v>
       </c>
-      <c r="K4" s="36">
+      <c r="K4" s="34">
         <v>60</v>
       </c>
-      <c r="L4" s="36">
+      <c r="L4" s="34">
         <v>60</v>
       </c>
-      <c r="M4" s="36">
+      <c r="M4" s="34">
         <v>60</v>
       </c>
-      <c r="N4" s="36">
+      <c r="N4" s="34">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="33"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
@@ -976,16 +1115,16 @@
       <c r="G5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="33"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
@@ -997,16 +1136,16 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="34"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
@@ -1014,16 +1153,16 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="36"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="35" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1037,30 +1176,30 @@
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="43">
-        <v>4</v>
-      </c>
-      <c r="I8" s="43">
+      <c r="H8" s="38">
+        <v>4</v>
+      </c>
+      <c r="I8" s="38">
         <v>2</v>
       </c>
-      <c r="J8" s="35">
+      <c r="J8" s="39">
         <v>40</v>
       </c>
-      <c r="K8" s="36">
+      <c r="K8" s="34">
         <v>60</v>
       </c>
-      <c r="L8" s="36">
+      <c r="L8" s="34">
         <v>60</v>
       </c>
-      <c r="M8" s="36">
+      <c r="M8" s="34">
         <v>60</v>
       </c>
-      <c r="N8" s="36">
+      <c r="N8" s="34">
         <v>60</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="33"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
@@ -1076,16 +1215,16 @@
       <c r="G9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="33"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
@@ -1097,16 +1236,16 @@
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="36"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="34"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
@@ -1114,16 +1253,16 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="36"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="35" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1137,30 +1276,30 @@
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="43">
-        <v>4</v>
-      </c>
-      <c r="I12" s="43">
+      <c r="H12" s="38">
+        <v>4</v>
+      </c>
+      <c r="I12" s="38">
         <v>2</v>
       </c>
-      <c r="J12" s="35">
+      <c r="J12" s="39">
         <v>40</v>
       </c>
-      <c r="K12" s="36">
+      <c r="K12" s="34">
         <v>60</v>
       </c>
-      <c r="L12" s="36">
+      <c r="L12" s="34">
         <v>60</v>
       </c>
-      <c r="M12" s="36">
+      <c r="M12" s="34">
         <v>60</v>
       </c>
-      <c r="N12" s="36">
+      <c r="N12" s="34">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="33"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1176,16 +1315,16 @@
       <c r="G13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="33"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="2" t="s">
         <v>23</v>
       </c>
@@ -1197,16 +1336,16 @@
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="34"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1214,16 +1353,26 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="L4:L7"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:N2"/>
+    <mergeCell ref="M4:M7"/>
+    <mergeCell ref="N4:N7"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="H4:H7"/>
     <mergeCell ref="L12:L15"/>
     <mergeCell ref="M12:M15"/>
     <mergeCell ref="N12:N15"/>
@@ -1240,16 +1389,6 @@
     <mergeCell ref="L8:L11"/>
     <mergeCell ref="M8:M11"/>
     <mergeCell ref="N8:N11"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="L4:L7"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:N2"/>
-    <mergeCell ref="M4:M7"/>
-    <mergeCell ref="N4:N7"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="H4:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1276,40 +1415,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="46"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="51"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="40" t="s">
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="42"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="45"/>
     </row>
     <row r="4" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
@@ -1353,7 +1492,7 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="46" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -1367,24 +1506,24 @@
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
-      <c r="H5" s="50">
+      <c r="H5" s="48">
         <v>6</v>
       </c>
-      <c r="I5" s="43">
+      <c r="I5" s="38">
         <v>2</v>
       </c>
-      <c r="J5" s="35">
+      <c r="J5" s="39">
         <v>100</v>
       </c>
-      <c r="K5" s="36">
+      <c r="K5" s="34">
         <v>60</v>
       </c>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
     </row>
     <row r="6" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="48"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="14" t="s">
         <v>2</v>
       </c>
@@ -1400,16 +1539,16 @@
       <c r="G6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="50"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
     </row>
     <row r="7" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="46" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -1423,22 +1562,22 @@
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="21"/>
-      <c r="H7" s="50">
+      <c r="H7" s="48">
         <v>8</v>
       </c>
-      <c r="I7" s="43">
-        <v>4</v>
-      </c>
-      <c r="J7" s="35">
+      <c r="I7" s="38">
+        <v>4</v>
+      </c>
+      <c r="J7" s="39">
         <v>100</v>
       </c>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="36"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
     </row>
     <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="48"/>
+      <c r="B8" s="47"/>
       <c r="C8" s="14" t="s">
         <v>2</v>
       </c>
@@ -1454,16 +1593,16 @@
       <c r="G8" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="50"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
     </row>
     <row r="9" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="46" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="15" t="s">
@@ -1477,22 +1616,22 @@
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="21"/>
-      <c r="H9" s="50">
+      <c r="H9" s="48">
         <v>8</v>
       </c>
-      <c r="I9" s="43">
-        <v>4</v>
-      </c>
-      <c r="J9" s="35">
+      <c r="I9" s="38">
+        <v>4</v>
+      </c>
+      <c r="J9" s="39">
         <v>60</v>
       </c>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
     </row>
     <row r="10" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="48"/>
+      <c r="B10" s="47"/>
       <c r="C10" s="14" t="s">
         <v>2</v>
       </c>
@@ -1508,16 +1647,16 @@
       <c r="G10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="50"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="36"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
     </row>
     <row r="11" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="46" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="15" t="s">
@@ -1531,30 +1670,30 @@
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="21"/>
-      <c r="H11" s="50">
+      <c r="H11" s="48">
         <v>8</v>
       </c>
-      <c r="I11" s="43">
-        <v>4</v>
-      </c>
-      <c r="J11" s="35">
+      <c r="I11" s="38">
+        <v>4</v>
+      </c>
+      <c r="J11" s="39">
         <v>60</v>
       </c>
-      <c r="K11" s="36">
+      <c r="K11" s="34">
         <v>50</v>
       </c>
-      <c r="L11" s="36">
+      <c r="L11" s="34">
         <v>50</v>
       </c>
-      <c r="M11" s="36">
+      <c r="M11" s="34">
         <v>50</v>
       </c>
-      <c r="N11" s="36">
+      <c r="N11" s="34">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="48"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="15" t="s">
         <v>2</v>
       </c>
@@ -1570,16 +1709,16 @@
       <c r="G12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="50"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
     </row>
     <row r="13" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="49"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="14" t="s">
         <v>23</v>
       </c>
@@ -1591,35 +1730,16 @@
       </c>
       <c r="F13" s="24"/>
       <c r="G13" s="25"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:N3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="N11:N13"/>
     <mergeCell ref="B2:N2"/>
@@ -1636,6 +1756,25 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:N3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -1646,7 +1785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1664,40 +1803,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="46"/>
+      <c r="B2" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="51"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="40" t="s">
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="42"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="45"/>
     </row>
     <row r="4" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
@@ -1741,11 +1880,11 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="46" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>13</v>
@@ -1755,26 +1894,26 @@
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
-      <c r="H5" s="50">
+      <c r="H5" s="48">
         <v>6</v>
       </c>
-      <c r="I5" s="43">
+      <c r="I5" s="38">
         <v>2</v>
       </c>
-      <c r="J5" s="35">
+      <c r="J5" s="39">
         <v>100</v>
       </c>
-      <c r="K5" s="36">
+      <c r="K5" s="34">
         <v>60</v>
       </c>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
     </row>
     <row r="6" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="48"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="27" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>16</v>
@@ -1788,16 +1927,16 @@
       <c r="G6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="50"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
     </row>
     <row r="7" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="46" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="28" t="s">
@@ -1811,22 +1950,22 @@
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="21"/>
-      <c r="H7" s="50">
+      <c r="H7" s="48">
         <v>8</v>
       </c>
-      <c r="I7" s="43">
-        <v>4</v>
-      </c>
-      <c r="J7" s="35">
+      <c r="I7" s="38">
+        <v>4</v>
+      </c>
+      <c r="J7" s="39">
         <v>100</v>
       </c>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="36"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
     </row>
     <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="48"/>
+      <c r="B8" s="47"/>
       <c r="C8" s="27" t="s">
         <v>40</v>
       </c>
@@ -1842,16 +1981,16 @@
       <c r="G8" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="50"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
     </row>
     <row r="9" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="46" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="28" t="s">
@@ -1865,22 +2004,22 @@
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="21"/>
-      <c r="H9" s="50">
+      <c r="H9" s="48">
         <v>8</v>
       </c>
-      <c r="I9" s="43">
-        <v>4</v>
-      </c>
-      <c r="J9" s="35">
+      <c r="I9" s="38">
+        <v>4</v>
+      </c>
+      <c r="J9" s="39">
         <v>60</v>
       </c>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
     </row>
     <row r="10" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="48"/>
+      <c r="B10" s="47"/>
       <c r="C10" s="27" t="s">
         <v>40</v>
       </c>
@@ -1896,16 +2035,16 @@
       <c r="G10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="50"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="36"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
     </row>
     <row r="11" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="46" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="28" t="s">
@@ -1919,30 +2058,30 @@
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="21"/>
-      <c r="H11" s="50">
+      <c r="H11" s="48">
         <v>8</v>
       </c>
-      <c r="I11" s="43">
-        <v>4</v>
-      </c>
-      <c r="J11" s="35">
+      <c r="I11" s="38">
+        <v>4</v>
+      </c>
+      <c r="J11" s="39">
         <v>60</v>
       </c>
-      <c r="K11" s="36">
+      <c r="K11" s="34">
         <v>50</v>
       </c>
-      <c r="L11" s="36">
+      <c r="L11" s="34">
         <v>50</v>
       </c>
-      <c r="M11" s="36">
+      <c r="M11" s="34">
         <v>50</v>
       </c>
-      <c r="N11" s="36">
+      <c r="N11" s="34">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="48"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="29" t="s">
         <v>40</v>
       </c>
@@ -1958,16 +2097,16 @@
       <c r="G12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="50"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
     </row>
     <row r="13" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="49"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="30" t="s">
         <v>41</v>
       </c>
@@ -1979,16 +2118,37 @@
       </c>
       <c r="F13" s="24"/>
       <c r="G13" s="25"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:N3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
     <mergeCell ref="L11:L13"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="N11:N13"/>
@@ -2003,25 +2163,495 @@
     <mergeCell ref="I11:I13"/>
     <mergeCell ref="J11:J13"/>
     <mergeCell ref="K11:K13"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:N3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:O16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" style="68" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="68" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="31" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="15" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="51"/>
+    </row>
+    <row r="3" spans="2:15" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="45"/>
+    </row>
+    <row r="4" spans="2:15" ht="33" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="57">
+        <v>6</v>
+      </c>
+      <c r="J5" s="57">
+        <v>2</v>
+      </c>
+      <c r="K5" s="70" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5" s="74" t="s">
+        <v>60</v>
+      </c>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+    </row>
+    <row r="6" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="36"/>
+      <c r="C6" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="29"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="71"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+    </row>
+    <row r="7" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="37"/>
+      <c r="C7" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="61" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="60"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="56"/>
+      <c r="O7" s="56"/>
+    </row>
+    <row r="8" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="57">
+        <v>4</v>
+      </c>
+      <c r="J8" s="57">
+        <v>2</v>
+      </c>
+      <c r="K8" s="69" t="s">
+        <v>59</v>
+      </c>
+      <c r="L8" s="74" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+    </row>
+    <row r="9" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="36"/>
+      <c r="C9" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="29"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="62"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="59"/>
+      <c r="N9" s="59"/>
+      <c r="O9" s="59"/>
+    </row>
+    <row r="10" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="37"/>
+      <c r="C10" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="60"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="56"/>
+      <c r="O10" s="56"/>
+    </row>
+    <row r="11" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="57">
+        <v>4</v>
+      </c>
+      <c r="J11" s="57">
+        <v>2</v>
+      </c>
+      <c r="K11" s="70" t="s">
+        <v>59</v>
+      </c>
+      <c r="L11" s="74" t="s">
+        <v>60</v>
+      </c>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+    </row>
+    <row r="12" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="36"/>
+      <c r="C12" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="29"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="73"/>
+      <c r="M12" s="59"/>
+      <c r="N12" s="59"/>
+      <c r="O12" s="59"/>
+    </row>
+    <row r="13" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="37"/>
+      <c r="C13" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="60"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="72"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="56"/>
+      <c r="N13" s="56"/>
+      <c r="O13" s="56"/>
+    </row>
+    <row r="14" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="32"/>
+      <c r="D14" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="28"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="48">
+        <v>8</v>
+      </c>
+      <c r="J14" s="38">
+        <v>4</v>
+      </c>
+      <c r="K14" s="70" t="s">
+        <v>59</v>
+      </c>
+      <c r="L14" s="74" t="s">
+        <v>60</v>
+      </c>
+      <c r="M14" s="74" t="s">
+        <v>60</v>
+      </c>
+      <c r="N14" s="74" t="s">
+        <v>60</v>
+      </c>
+      <c r="O14" s="74" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="47"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="64" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="48"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="71"/>
+      <c r="L15" s="73"/>
+      <c r="M15" s="73"/>
+      <c r="N15" s="73"/>
+      <c r="O15" s="73"/>
+    </row>
+    <row r="16" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="52"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="30"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="72"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="54"/>
+      <c r="O16" s="54"/>
+    </row>
+  </sheetData>
+  <mergeCells count="35">
+    <mergeCell ref="L5:L7"/>
+    <mergeCell ref="K5:K7"/>
+    <mergeCell ref="L8:L10"/>
+    <mergeCell ref="L11:L13"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="J5:J7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="K14:K16"/>
+    <mergeCell ref="L14:L16"/>
+    <mergeCell ref="M14:M16"/>
+    <mergeCell ref="N14:N16"/>
+    <mergeCell ref="O14:O16"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="I3:O3"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
   </mergeCells>

</xml_diff>

<commit_message>
update tai lieu queens
update tai lieu queens
</commit_message>
<xml_diff>
--- a/tools/IP-Planning-Hardware-Requirements.xlsx
+++ b/tools/IP-Planning-Hardware-Requirements.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CEPH-Alone" sheetId="7" r:id="rId1"/>
     <sheet name="OpenStack_Ceph-AIO-Ubuntu" sheetId="8" r:id="rId2"/>
     <sheet name="OpenStack_Ceph-AIO-CentOS" sheetId="9" r:id="rId3"/>
     <sheet name="OpenStack_Pike" sheetId="10" r:id="rId4"/>
+    <sheet name="OpenStack_Queens" sheetId="11" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="78">
   <si>
     <t>Controller</t>
   </si>
@@ -228,6 +229,45 @@
   </si>
   <si>
     <t>NAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bridge</t>
+  </si>
+  <si>
+    <t>10.10.10.201</t>
+  </si>
+  <si>
+    <t>172.16.68.201</t>
+  </si>
+  <si>
+    <t>192.168.20.201</t>
+  </si>
+  <si>
+    <t>10.10.10.202</t>
+  </si>
+  <si>
+    <t>172.16.68.202</t>
+  </si>
+  <si>
+    <t>192.168.20.202</t>
+  </si>
+  <si>
+    <t>10.10.10.203</t>
+  </si>
+  <si>
+    <t>172.16.68.203</t>
+  </si>
+  <si>
+    <t>192.168.20.203</t>
+  </si>
+  <si>
+    <t>Controller1</t>
+  </si>
+  <si>
+    <t>172.16.68.1</t>
+  </si>
+  <si>
+    <t>IP PLANNING - OpenStack Queens</t>
   </si>
 </sst>
 </file>
@@ -489,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -580,82 +620,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -664,9 +638,6 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -685,22 +656,97 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1002,23 +1048,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="43" t="s">
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="45"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="56"/>
     </row>
     <row r="3" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
@@ -1062,7 +1108,7 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="46" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1076,30 +1122,30 @@
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="38">
-        <v>4</v>
-      </c>
-      <c r="I4" s="38">
+      <c r="H4" s="57">
+        <v>4</v>
+      </c>
+      <c r="I4" s="57">
         <v>2</v>
       </c>
-      <c r="J4" s="39">
+      <c r="J4" s="49">
         <v>40</v>
       </c>
-      <c r="K4" s="34">
+      <c r="K4" s="50">
         <v>60</v>
       </c>
-      <c r="L4" s="34">
+      <c r="L4" s="50">
         <v>60</v>
       </c>
-      <c r="M4" s="34">
+      <c r="M4" s="50">
         <v>60</v>
       </c>
-      <c r="N4" s="34">
+      <c r="N4" s="50">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="36"/>
+      <c r="B5" s="47"/>
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
@@ -1115,16 +1161,16 @@
       <c r="G5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="36"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
@@ -1136,16 +1182,16 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="37"/>
+      <c r="B7" s="48"/>
       <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
@@ -1153,16 +1199,16 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="46" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1176,30 +1222,30 @@
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="38">
-        <v>4</v>
-      </c>
-      <c r="I8" s="38">
+      <c r="H8" s="57">
+        <v>4</v>
+      </c>
+      <c r="I8" s="57">
         <v>2</v>
       </c>
-      <c r="J8" s="39">
+      <c r="J8" s="49">
         <v>40</v>
       </c>
-      <c r="K8" s="34">
+      <c r="K8" s="50">
         <v>60</v>
       </c>
-      <c r="L8" s="34">
+      <c r="L8" s="50">
         <v>60</v>
       </c>
-      <c r="M8" s="34">
+      <c r="M8" s="50">
         <v>60</v>
       </c>
-      <c r="N8" s="34">
+      <c r="N8" s="50">
         <v>60</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="36"/>
+      <c r="B9" s="47"/>
       <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
@@ -1215,16 +1261,16 @@
       <c r="G9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="50"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="36"/>
+      <c r="B10" s="47"/>
       <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
@@ -1236,16 +1282,16 @@
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="37"/>
+      <c r="B11" s="48"/>
       <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
@@ -1253,16 +1299,16 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="46" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1276,30 +1322,30 @@
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="38">
-        <v>4</v>
-      </c>
-      <c r="I12" s="38">
+      <c r="H12" s="57">
+        <v>4</v>
+      </c>
+      <c r="I12" s="57">
         <v>2</v>
       </c>
-      <c r="J12" s="39">
+      <c r="J12" s="49">
         <v>40</v>
       </c>
-      <c r="K12" s="34">
+      <c r="K12" s="50">
         <v>60</v>
       </c>
-      <c r="L12" s="34">
+      <c r="L12" s="50">
         <v>60</v>
       </c>
-      <c r="M12" s="34">
+      <c r="M12" s="50">
         <v>60</v>
       </c>
-      <c r="N12" s="34">
+      <c r="N12" s="50">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="36"/>
+      <c r="B13" s="47"/>
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1315,16 +1361,16 @@
       <c r="G13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="50"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="36"/>
+      <c r="B14" s="47"/>
       <c r="C14" s="2" t="s">
         <v>23</v>
       </c>
@@ -1336,16 +1382,16 @@
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="50"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="37"/>
+      <c r="B15" s="48"/>
       <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1353,26 +1399,16 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="L4:L7"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:N2"/>
-    <mergeCell ref="M4:M7"/>
-    <mergeCell ref="N4:N7"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="H4:H7"/>
     <mergeCell ref="L12:L15"/>
     <mergeCell ref="M12:M15"/>
     <mergeCell ref="N12:N15"/>
@@ -1389,6 +1425,16 @@
     <mergeCell ref="L8:L11"/>
     <mergeCell ref="M8:M11"/>
     <mergeCell ref="N8:N11"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="L4:L7"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:N2"/>
+    <mergeCell ref="M4:M7"/>
+    <mergeCell ref="N4:N7"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="H4:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1415,40 +1461,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="51"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="60"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="43" t="s">
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="45"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="56"/>
     </row>
     <row r="4" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
@@ -1492,7 +1538,7 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="61" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -1506,24 +1552,24 @@
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
-      <c r="H5" s="48">
+      <c r="H5" s="64">
         <v>6</v>
       </c>
-      <c r="I5" s="38">
+      <c r="I5" s="57">
         <v>2</v>
       </c>
-      <c r="J5" s="39">
+      <c r="J5" s="49">
         <v>100</v>
       </c>
-      <c r="K5" s="34">
+      <c r="K5" s="50">
         <v>60</v>
       </c>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
     </row>
     <row r="6" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="47"/>
+      <c r="B6" s="62"/>
       <c r="C6" s="14" t="s">
         <v>2</v>
       </c>
@@ -1539,16 +1585,16 @@
       <c r="G6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="48"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
     </row>
     <row r="7" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="61" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -1562,22 +1608,22 @@
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="21"/>
-      <c r="H7" s="48">
+      <c r="H7" s="64">
         <v>8</v>
       </c>
-      <c r="I7" s="38">
-        <v>4</v>
-      </c>
-      <c r="J7" s="39">
+      <c r="I7" s="57">
+        <v>4</v>
+      </c>
+      <c r="J7" s="49">
         <v>100</v>
       </c>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
     </row>
     <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="47"/>
+      <c r="B8" s="62"/>
       <c r="C8" s="14" t="s">
         <v>2</v>
       </c>
@@ -1593,16 +1639,16 @@
       <c r="G8" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="48"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
     </row>
     <row r="9" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="61" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="15" t="s">
@@ -1616,22 +1662,22 @@
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="21"/>
-      <c r="H9" s="48">
+      <c r="H9" s="64">
         <v>8</v>
       </c>
-      <c r="I9" s="38">
-        <v>4</v>
-      </c>
-      <c r="J9" s="39">
+      <c r="I9" s="57">
+        <v>4</v>
+      </c>
+      <c r="J9" s="49">
         <v>60</v>
       </c>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="50"/>
     </row>
     <row r="10" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="47"/>
+      <c r="B10" s="62"/>
       <c r="C10" s="14" t="s">
         <v>2</v>
       </c>
@@ -1647,16 +1693,16 @@
       <c r="G10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="48"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
     </row>
     <row r="11" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="61" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="15" t="s">
@@ -1670,30 +1716,30 @@
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="21"/>
-      <c r="H11" s="48">
+      <c r="H11" s="64">
         <v>8</v>
       </c>
-      <c r="I11" s="38">
-        <v>4</v>
-      </c>
-      <c r="J11" s="39">
+      <c r="I11" s="57">
+        <v>4</v>
+      </c>
+      <c r="J11" s="49">
         <v>60</v>
       </c>
-      <c r="K11" s="34">
+      <c r="K11" s="50">
         <v>50</v>
       </c>
-      <c r="L11" s="34">
+      <c r="L11" s="50">
         <v>50</v>
       </c>
-      <c r="M11" s="34">
+      <c r="M11" s="50">
         <v>50</v>
       </c>
-      <c r="N11" s="34">
+      <c r="N11" s="50">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="47"/>
+      <c r="B12" s="62"/>
       <c r="C12" s="15" t="s">
         <v>2</v>
       </c>
@@ -1709,16 +1755,16 @@
       <c r="G12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="48"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
     </row>
     <row r="13" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="52"/>
+      <c r="B13" s="63"/>
       <c r="C13" s="14" t="s">
         <v>23</v>
       </c>
@@ -1730,16 +1776,35 @@
       </c>
       <c r="F13" s="24"/>
       <c r="G13" s="25"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:N3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="N11:N13"/>
     <mergeCell ref="B2:N2"/>
@@ -1756,25 +1821,6 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:N3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -1803,40 +1849,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="51"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="60"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="43" t="s">
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="45"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="56"/>
     </row>
     <row r="4" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
@@ -1880,7 +1926,7 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="61" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="26" t="s">
@@ -1894,24 +1940,24 @@
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
-      <c r="H5" s="48">
+      <c r="H5" s="64">
         <v>6</v>
       </c>
-      <c r="I5" s="38">
+      <c r="I5" s="57">
         <v>2</v>
       </c>
-      <c r="J5" s="39">
+      <c r="J5" s="49">
         <v>100</v>
       </c>
-      <c r="K5" s="34">
+      <c r="K5" s="50">
         <v>60</v>
       </c>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
     </row>
     <row r="6" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="47"/>
+      <c r="B6" s="62"/>
       <c r="C6" s="27" t="s">
         <v>47</v>
       </c>
@@ -1927,16 +1973,16 @@
       <c r="G6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="48"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
     </row>
     <row r="7" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="61" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="28" t="s">
@@ -1950,22 +1996,22 @@
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="21"/>
-      <c r="H7" s="48">
+      <c r="H7" s="64">
         <v>8</v>
       </c>
-      <c r="I7" s="38">
-        <v>4</v>
-      </c>
-      <c r="J7" s="39">
+      <c r="I7" s="57">
+        <v>4</v>
+      </c>
+      <c r="J7" s="49">
         <v>100</v>
       </c>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
     </row>
     <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="47"/>
+      <c r="B8" s="62"/>
       <c r="C8" s="27" t="s">
         <v>40</v>
       </c>
@@ -1981,16 +2027,16 @@
       <c r="G8" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="48"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
     </row>
     <row r="9" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="61" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="28" t="s">
@@ -2004,22 +2050,22 @@
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="21"/>
-      <c r="H9" s="48">
+      <c r="H9" s="64">
         <v>8</v>
       </c>
-      <c r="I9" s="38">
-        <v>4</v>
-      </c>
-      <c r="J9" s="39">
+      <c r="I9" s="57">
+        <v>4</v>
+      </c>
+      <c r="J9" s="49">
         <v>60</v>
       </c>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="50"/>
     </row>
     <row r="10" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="47"/>
+      <c r="B10" s="62"/>
       <c r="C10" s="27" t="s">
         <v>40</v>
       </c>
@@ -2035,16 +2081,16 @@
       <c r="G10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="48"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
     </row>
     <row r="11" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="61" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="28" t="s">
@@ -2058,30 +2104,30 @@
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="21"/>
-      <c r="H11" s="48">
+      <c r="H11" s="64">
         <v>8</v>
       </c>
-      <c r="I11" s="38">
-        <v>4</v>
-      </c>
-      <c r="J11" s="39">
+      <c r="I11" s="57">
+        <v>4</v>
+      </c>
+      <c r="J11" s="49">
         <v>60</v>
       </c>
-      <c r="K11" s="34">
+      <c r="K11" s="50">
         <v>50</v>
       </c>
-      <c r="L11" s="34">
+      <c r="L11" s="50">
         <v>50</v>
       </c>
-      <c r="M11" s="34">
+      <c r="M11" s="50">
         <v>50</v>
       </c>
-      <c r="N11" s="34">
+      <c r="N11" s="50">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="47"/>
+      <c r="B12" s="62"/>
       <c r="C12" s="29" t="s">
         <v>40</v>
       </c>
@@ -2097,16 +2143,16 @@
       <c r="G12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="48"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
     </row>
     <row r="13" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="52"/>
+      <c r="B13" s="63"/>
       <c r="C13" s="30" t="s">
         <v>41</v>
       </c>
@@ -2118,37 +2164,16 @@
       </c>
       <c r="F13" s="24"/>
       <c r="G13" s="25"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:N3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
     <mergeCell ref="L11:L13"/>
     <mergeCell ref="M11:M13"/>
     <mergeCell ref="N11:N13"/>
@@ -2163,6 +2188,27 @@
     <mergeCell ref="I11:I13"/>
     <mergeCell ref="J11:J13"/>
     <mergeCell ref="K11:K13"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:N3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -2173,8 +2219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2183,8 +2229,8 @@
     <col min="3" max="3" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" style="31" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" style="68" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="68" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" style="45" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="45" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" style="31" customWidth="1"/>
     <col min="9" max="9" width="7.140625" style="3" customWidth="1"/>
     <col min="10" max="10" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
@@ -2192,42 +2238,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="51"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="60"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="43" t="s">
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="45"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="56"/>
     </row>
     <row r="4" spans="2:15" ht="33" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
@@ -2274,7 +2320,7 @@
       </c>
     </row>
     <row r="5" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="46" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="26" t="s">
@@ -2292,27 +2338,27 @@
       <c r="G5" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="63" t="s">
+      <c r="H5" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="57">
+      <c r="I5" s="71">
         <v>6</v>
       </c>
-      <c r="J5" s="57">
+      <c r="J5" s="71">
         <v>2</v>
       </c>
-      <c r="K5" s="70" t="s">
+      <c r="K5" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="L5" s="74" t="s">
+      <c r="L5" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
     </row>
     <row r="6" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="36"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="29" t="s">
         <v>63</v>
       </c>
@@ -2326,41 +2372,41 @@
         <v>4</v>
       </c>
       <c r="G6" s="29"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="59"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="74"/>
+      <c r="N6" s="74"/>
+      <c r="O6" s="74"/>
     </row>
     <row r="7" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="37"/>
-      <c r="C7" s="60" t="s">
+      <c r="B7" s="48"/>
+      <c r="C7" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="D7" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="61" t="s">
+      <c r="E7" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="60"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="56"/>
-      <c r="N7" s="56"/>
-      <c r="O7" s="56"/>
+      <c r="F7" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="38"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
     </row>
     <row r="8" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="46" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="26" t="s">
@@ -2378,27 +2424,27 @@
       <c r="G8" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="63" t="s">
+      <c r="H8" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="57">
-        <v>4</v>
-      </c>
-      <c r="J8" s="57">
+      <c r="I8" s="71">
+        <v>4</v>
+      </c>
+      <c r="J8" s="71">
         <v>2</v>
       </c>
-      <c r="K8" s="69" t="s">
+      <c r="K8" s="75" t="s">
         <v>59</v>
       </c>
-      <c r="L8" s="74" t="s">
+      <c r="L8" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="50"/>
     </row>
     <row r="9" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="36"/>
+      <c r="B9" s="47"/>
       <c r="C9" s="29" t="s">
         <v>63</v>
       </c>
@@ -2412,41 +2458,41 @@
         <v>4</v>
       </c>
       <c r="G9" s="29"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="62"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="73"/>
-      <c r="M9" s="59"/>
-      <c r="N9" s="59"/>
-      <c r="O9" s="59"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="74"/>
+      <c r="N9" s="74"/>
+      <c r="O9" s="74"/>
     </row>
     <row r="10" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="37"/>
-      <c r="C10" s="60" t="s">
+      <c r="B10" s="48"/>
+      <c r="C10" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="60" t="s">
+      <c r="D10" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="61" t="s">
+      <c r="E10" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" s="60"/>
-      <c r="H10" s="65"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="54"/>
-      <c r="M10" s="56"/>
-      <c r="N10" s="56"/>
-      <c r="O10" s="56"/>
+      <c r="F10" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="38"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="67"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
     </row>
     <row r="11" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="46" t="s">
         <v>36</v>
       </c>
       <c r="C11" s="26" t="s">
@@ -2464,27 +2510,27 @@
       <c r="G11" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="63" t="s">
+      <c r="H11" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="57">
-        <v>4</v>
-      </c>
-      <c r="J11" s="57">
+      <c r="I11" s="71">
+        <v>4</v>
+      </c>
+      <c r="J11" s="71">
         <v>2</v>
       </c>
-      <c r="K11" s="70" t="s">
+      <c r="K11" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="L11" s="74" t="s">
+      <c r="L11" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="50"/>
     </row>
     <row r="12" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="36"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="29" t="s">
         <v>63</v>
       </c>
@@ -2498,41 +2544,41 @@
         <v>4</v>
       </c>
       <c r="G12" s="29"/>
-      <c r="H12" s="64"/>
-      <c r="I12" s="62"/>
-      <c r="J12" s="62"/>
-      <c r="K12" s="71"/>
-      <c r="L12" s="73"/>
-      <c r="M12" s="59"/>
-      <c r="N12" s="59"/>
-      <c r="O12" s="59"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="69"/>
+      <c r="L12" s="66"/>
+      <c r="M12" s="74"/>
+      <c r="N12" s="74"/>
+      <c r="O12" s="74"/>
     </row>
     <row r="13" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="37"/>
-      <c r="C13" s="60" t="s">
+      <c r="B13" s="48"/>
+      <c r="C13" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="60" t="s">
+      <c r="D13" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="61" t="s">
+      <c r="E13" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="G13" s="60"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="72"/>
-      <c r="L13" s="54"/>
-      <c r="M13" s="56"/>
-      <c r="N13" s="56"/>
-      <c r="O13" s="56"/>
+      <c r="F13" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="38"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="70"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
     </row>
     <row r="14" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="61" t="s">
         <v>37</v>
       </c>
       <c r="C14" s="32"/>
@@ -2546,31 +2592,31 @@
         <v>4</v>
       </c>
       <c r="G14" s="28"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="48">
+      <c r="H14" s="43"/>
+      <c r="I14" s="64">
         <v>8</v>
       </c>
-      <c r="J14" s="38">
-        <v>4</v>
-      </c>
-      <c r="K14" s="70" t="s">
+      <c r="J14" s="57">
+        <v>4</v>
+      </c>
+      <c r="K14" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="L14" s="74" t="s">
+      <c r="L14" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="M14" s="74" t="s">
+      <c r="M14" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="N14" s="74" t="s">
+      <c r="N14" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="O14" s="74" t="s">
+      <c r="O14" s="65" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="47"/>
+      <c r="B15" s="62"/>
       <c r="C15" s="32"/>
       <c r="D15" s="29" t="s">
         <v>40</v>
@@ -2584,19 +2630,19 @@
       <c r="G15" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="64" t="s">
+      <c r="H15" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="48"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="71"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="73"/>
-      <c r="N15" s="73"/>
-      <c r="O15" s="73"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="66"/>
+      <c r="M15" s="66"/>
+      <c r="N15" s="66"/>
+      <c r="O15" s="66"/>
     </row>
     <row r="16" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="52"/>
+      <c r="B16" s="63"/>
       <c r="C16" s="33"/>
       <c r="D16" s="30" t="s">
         <v>41</v>
@@ -2608,29 +2654,28 @@
         <v>4</v>
       </c>
       <c r="G16" s="30"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="72"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="54"/>
-      <c r="O16" s="54"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="L5:L7"/>
-    <mergeCell ref="K5:K7"/>
-    <mergeCell ref="L8:L10"/>
-    <mergeCell ref="L11:L13"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="J5:J7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="J8:J10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
     <mergeCell ref="N11:N12"/>
     <mergeCell ref="O11:O12"/>
     <mergeCell ref="B14:B16"/>
@@ -2643,15 +2688,471 @@
     <mergeCell ref="O14:O16"/>
     <mergeCell ref="M11:M12"/>
     <mergeCell ref="K11:K13"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="L5:L7"/>
+    <mergeCell ref="K5:K7"/>
+    <mergeCell ref="L8:L10"/>
+    <mergeCell ref="L11:L13"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="J5:J7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:O16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" style="45" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="45" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="31" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="15" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="60"/>
+    </row>
+    <row r="3" spans="2:15" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="56"/>
+    </row>
+    <row r="4" spans="2:15" ht="33" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="26"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="71">
+        <v>6</v>
+      </c>
+      <c r="J5" s="71">
+        <v>2</v>
+      </c>
+      <c r="K5" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+    </row>
+    <row r="6" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="47"/>
+      <c r="C6" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="74"/>
+      <c r="N6" s="74"/>
+      <c r="O6" s="74"/>
+    </row>
+    <row r="7" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="48"/>
+      <c r="C7" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="38"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+    </row>
+    <row r="8" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="26"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="71">
+        <v>4</v>
+      </c>
+      <c r="J8" s="71">
+        <v>2</v>
+      </c>
+      <c r="K8" s="75" t="s">
+        <v>59</v>
+      </c>
+      <c r="L8" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="50"/>
+    </row>
+    <row r="9" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="47"/>
+      <c r="C9" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="72"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="74"/>
+      <c r="N9" s="74"/>
+      <c r="O9" s="74"/>
+    </row>
+    <row r="10" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="48"/>
+      <c r="C10" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="38"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="67"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
+    </row>
+    <row r="11" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="40"/>
+      <c r="I11" s="71">
+        <v>4</v>
+      </c>
+      <c r="J11" s="71">
+        <v>2</v>
+      </c>
+      <c r="K11" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="L11" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="50"/>
+    </row>
+    <row r="12" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="47"/>
+      <c r="C12" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="29"/>
+      <c r="H12" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="72"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="69"/>
+      <c r="L12" s="66"/>
+      <c r="M12" s="74"/>
+      <c r="N12" s="74"/>
+      <c r="O12" s="74"/>
+    </row>
+    <row r="13" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="48"/>
+      <c r="C13" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="38"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="70"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+    </row>
+    <row r="14" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="68"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="65"/>
+      <c r="N14" s="65"/>
+      <c r="O14" s="65"/>
+    </row>
+    <row r="15" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="62"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="66"/>
+      <c r="M15" s="66"/>
+      <c r="N15" s="66"/>
+      <c r="O15" s="66"/>
+    </row>
+    <row r="16" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="63"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="67"/>
+    </row>
+  </sheetData>
+  <mergeCells count="35">
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="K14:K16"/>
+    <mergeCell ref="L14:L16"/>
+    <mergeCell ref="M14:M16"/>
+    <mergeCell ref="N14:N16"/>
+    <mergeCell ref="O14:O16"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="L11:L13"/>
+    <mergeCell ref="M11:M12"/>
     <mergeCell ref="O5:O6"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="J8:J10"/>
     <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L10"/>
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="N8:N9"/>
     <mergeCell ref="O8:O9"/>
-    <mergeCell ref="B5:B7"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="I3:O3"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="J5:J7"/>
+    <mergeCell ref="K5:K7"/>
+    <mergeCell ref="L5:L7"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
   </mergeCells>

</xml_diff>